<commit_message>
AutoDS Mise au point tests unitégration optimisation / optimiser + affinage traces + suite améliorations log
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1036B2-BACF-4219-92B1-2E139110173C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650B71A1-2E76-4F45-B1DB-FE395AC4534D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Echant1_impl" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>TrDrte</t>
   </si>
   <si>
-    <t>NbTrches</t>
-  </si>
-  <si>
     <t>Luscinia megarhynchos</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>10mn</t>
+  </si>
+  <si>
+    <t>NbTrchMod</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -465,7 +465,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -534,26 +534,26 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -578,10 +578,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,11 +618,12 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -631,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -640,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -654,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -668,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -685,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -702,7 +703,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -722,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -745,7 +746,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -759,7 +760,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -776,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>280</v>
@@ -793,7 +794,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -813,7 +814,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -836,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -850,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -867,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>280</v>
@@ -884,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -904,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -927,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -941,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18">
         <v>450</v>
@@ -958,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19">
         <v>500</v>
@@ -978,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -992,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <v>500</v>
@@ -1009,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22">
         <v>600</v>
@@ -1027,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A5133-9B74-4D19-823B-523AF343B54A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,11 +1040,12 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1052,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -1061,35 +1063,35 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1097,16 +1099,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -1114,16 +1116,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1137,30 +1139,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -1168,16 +1170,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>350</v>
@@ -1185,16 +1187,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>15</v>

</xml_diff>

<commit_message>
AutoDS Cohérence jeu test validation ACDC Extrait + non régression complète + tests optimiser sauf comparaison résultats à référence (à faire)
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650B71A1-2E76-4F45-B1DB-FE395AC4534D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F8BE8-65B3-4A11-913F-522D9470DD13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="20">
   <si>
     <t>Passage</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Turdus merula</t>
-  </si>
-  <si>
-    <t>m+a</t>
   </si>
   <si>
     <t>HNORMAL</t>
@@ -452,7 +449,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,7 +462,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -474,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -488,18 +485,15 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +519,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -534,26 +528,26 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -578,23 +572,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -604,10 +598,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A12" sqref="A12:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +617,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -632,16 +626,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -655,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -669,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -686,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -703,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -723,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -746,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -760,7 +754,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -777,7 +771,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>280</v>
@@ -794,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -814,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -828,93 +822,84 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>450</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14">
-        <v>280</v>
+        <v>500</v>
+      </c>
+      <c r="G14">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
-      <c r="F15">
-        <v>300</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16">
-        <v>300</v>
-      </c>
-      <c r="G16">
-        <v>19</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -930,92 +915,10 @@
       <c r="D17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19">
-        <v>500</v>
-      </c>
-      <c r="G19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22">
+      <c r="F17">
         <v>600</v>
       </c>
-      <c r="G22">
+      <c r="G17">
         <v>18</v>
       </c>
     </row>
@@ -1029,7 +932,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +948,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1054,44 +957,44 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1099,16 +1002,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -1116,16 +1019,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1139,30 +1042,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -1170,16 +1073,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>350</v>
@@ -1187,16 +1090,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>15</v>

</xml_diff>

<commit_message>
AutoDS Proto enchaint auto optim + analyses => futur MCDSOptanalyser
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eCloud\DistanceSampling\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F8BE8-65B3-4A11-913F-522D9470DD13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC30DD-9CA4-41A0-B345-6F1FAC37EA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Echant1_impl" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Modl_impl" sheetId="2" r:id="rId3"/>
     <sheet name="Params1_expl" sheetId="3" r:id="rId4"/>
     <sheet name="Params2_expl" sheetId="5" r:id="rId5"/>
+    <sheet name="Params3_expl" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="25">
   <si>
     <t>Passage</t>
   </si>
@@ -84,6 +85,21 @@
   </si>
   <si>
     <t>NbTrchMod</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>times(2)</t>
+  </si>
+  <si>
+    <t>times(3, b=2)</t>
+  </si>
+  <si>
+    <t>times(4)</t>
+  </si>
+  <si>
+    <t>MultiOpt</t>
   </si>
 </sst>
 </file>
@@ -449,18 +465,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -474,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -488,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -509,15 +525,15 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -531,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -545,7 +561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>18</v>
       </c>
@@ -561,16 +577,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -578,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -586,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -598,24 +614,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -637,8 +653,11 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -652,7 +671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -669,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -686,7 +705,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -706,7 +725,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -729,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -743,7 +762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -760,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -777,7 +796,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -797,7 +816,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -820,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -834,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -851,7 +870,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -871,7 +890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -885,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -902,7 +921,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -929,24 +948,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A5133-9B74-4D19-823B-523AF343B54A}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -968,8 +987,11 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -983,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1000,7 +1022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1017,7 +1039,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1040,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1110,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1111,4 +1133,185 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B23091B-ECC4-4DEB-9AF9-B2657F5DC316}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AutoDS Analyser: auto-explicitation + reconnaissance colonnes specs analyse dans run + extraction classe Analyser=base(DSAnalyser)
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-ExtraitSpecsAnalyses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eCloud\DistanceSampling\autods\refin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC30DD-9CA4-41A0-B345-6F1FAC37EA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3E423D-2DBD-4671-899C-9D29025EB125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13965" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Echant1_impl" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,13 @@
     <sheet name="Modl_impl" sheetId="2" r:id="rId3"/>
     <sheet name="Params1_expl" sheetId="3" r:id="rId4"/>
     <sheet name="Params2_expl" sheetId="5" r:id="rId5"/>
-    <sheet name="Params3_expl" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="20">
   <si>
     <t>Passage</t>
   </si>
@@ -85,21 +84,6 @@
   </si>
   <si>
     <t>NbTrchMod</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>times(2)</t>
-  </si>
-  <si>
-    <t>times(3, b=2)</t>
-  </si>
-  <si>
-    <t>times(4)</t>
-  </si>
-  <si>
-    <t>MultiOpt</t>
   </si>
 </sst>
 </file>
@@ -614,10 +598,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +615,7 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -653,11 +637,8 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -671,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -688,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -705,7 +686,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -725,7 +706,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -748,7 +729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -762,7 +743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -779,7 +760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -796,7 +777,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -816,7 +797,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -839,7 +820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -853,7 +834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -870,7 +851,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -890,7 +871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -904,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -948,10 +929,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A5133-9B74-4D19-823B-523AF343B54A}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +946,7 @@
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -987,11 +968,8 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1005,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1017,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1093,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1110,7 +1088,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1133,185 +1111,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B23091B-ECC4-4DEB-9AF9-B2657F5DC316}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>